<commit_message>
Add estimate to power allocation simulation
</commit_message>
<xml_diff>
--- a/configs-matlab.xlsx
+++ b/configs-matlab.xlsx
@@ -1,23 +1,27 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sshafaamri\Downloads\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="144" windowWidth="22980" windowHeight="8760" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12300"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
-    <sheet name="Sheet4" sheetId="4" r:id="rId4"/>
   </sheets>
-  <calcPr calcId="144525"/>
+  <calcPr calcId="162913"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="125" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="114" uniqueCount="24">
   <si>
     <t>#1</t>
   </si>
@@ -94,7 +98,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -138,6 +142,9 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -186,7 +193,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -221,7 +228,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -430,15 +437,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:M14"/>
+  <dimension ref="A1:N9"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="M14" sqref="M14"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F12" sqref="F12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>7</v>
       </c>
@@ -460,14 +467,14 @@
       <c r="I1" s="1"/>
       <c r="J1" s="1"/>
       <c r="K1" s="1"/>
-      <c r="L1" t="s">
+      <c r="M1" t="s">
         <v>22</v>
       </c>
-      <c r="M1" t="s">
+      <c r="N1" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>8</v>
       </c>
@@ -496,16 +503,19 @@
         <v>4</v>
       </c>
       <c r="K2" t="s">
+        <v>19</v>
+      </c>
+      <c r="L2" t="s">
         <v>5</v>
       </c>
-      <c r="L2" t="s">
+      <c r="M2" t="s">
         <v>0</v>
       </c>
-      <c r="M2">
+      <c r="N2">
         <v>6.5</v>
       </c>
     </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>9</v>
       </c>
@@ -537,16 +547,19 @@
         <v>0.78925144674350534</v>
       </c>
       <c r="K3">
+        <v>0.84873517670409704</v>
+      </c>
+      <c r="L3">
         <v>0.66693318927175926</v>
       </c>
-      <c r="L3" t="s">
+      <c r="M3" t="s">
         <v>1</v>
       </c>
-      <c r="M3">
+      <c r="N3">
         <v>6.5</v>
       </c>
     </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>10</v>
       </c>
@@ -578,16 +591,19 @@
         <v>0.68414733421793628</v>
       </c>
       <c r="K4">
+        <v>0.90976025235116076</v>
+      </c>
+      <c r="L4">
         <v>0.56134184814611221</v>
       </c>
-      <c r="L4" t="s">
+      <c r="M4" t="s">
         <v>2</v>
       </c>
-      <c r="M4">
+      <c r="N4">
         <v>6.5</v>
       </c>
     </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>11</v>
       </c>
@@ -619,27 +635,30 @@
         <v>0.75194091898838689</v>
       </c>
       <c r="K5">
+        <v>0.80393718277079063</v>
+      </c>
+      <c r="L5">
         <v>0.66055949079149767</v>
       </c>
-      <c r="L5" t="s">
+      <c r="M5" t="s">
         <v>3</v>
       </c>
-      <c r="M5">
+      <c r="N5">
         <v>6.5</v>
       </c>
     </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>12</v>
+        <v>20</v>
       </c>
       <c r="B6">
-        <v>45.414999999999999</v>
+        <v>46.045000000000002</v>
       </c>
       <c r="C6" t="s">
-        <v>18</v>
+        <v>21</v>
       </c>
       <c r="D6">
-        <v>4.1801275510204094</v>
+        <v>17.205841836734724</v>
       </c>
       <c r="E6" t="s">
         <v>3</v>
@@ -660,16 +679,31 @@
         <v>0.77003273234291192</v>
       </c>
       <c r="K6">
+        <v>0.75938414153647349</v>
+      </c>
+      <c r="L6">
         <v>0.65724787719077571</v>
       </c>
-      <c r="L6" t="s">
+      <c r="M6" t="s">
         <v>4</v>
       </c>
-      <c r="M6">
+      <c r="N6">
         <v>6.5</v>
       </c>
     </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>12</v>
+      </c>
+      <c r="B7">
+        <v>45.414999999999999</v>
+      </c>
+      <c r="C7" t="s">
+        <v>18</v>
+      </c>
+      <c r="D7">
+        <v>4.1801275510204094</v>
+      </c>
       <c r="E7" t="s">
         <v>4</v>
       </c>
@@ -689,42 +723,74 @@
         <v>4.9026530612244992</v>
       </c>
       <c r="K7">
+        <v>0.77261175598796694</v>
+      </c>
+      <c r="L7">
         <v>0.64701382882915426</v>
       </c>
-      <c r="L7" t="s">
+      <c r="M7" t="s">
         <v>19</v>
       </c>
-      <c r="M7">
+      <c r="N7">
         <v>6.5</v>
       </c>
     </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:14" x14ac:dyDescent="0.25">
       <c r="E8" t="s">
+        <v>19</v>
+      </c>
+      <c r="F8">
+        <v>0.84873517670409704</v>
+      </c>
+      <c r="G8">
+        <v>0.90976025235116076</v>
+      </c>
+      <c r="H8">
+        <v>0.80393718277079063</v>
+      </c>
+      <c r="I8">
+        <v>0.75938414153647349</v>
+      </c>
+      <c r="J8">
+        <v>0.77261175598796694</v>
+      </c>
+      <c r="K8">
+        <v>17.205841836734724</v>
+      </c>
+      <c r="L8">
+        <v>0.70087846409313204</v>
+      </c>
+      <c r="M8" t="s">
         <v>5</v>
       </c>
-      <c r="F8">
+      <c r="N8">
+        <v>6.5</v>
+      </c>
+    </row>
+    <row r="9" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="E9" t="s">
+        <v>5</v>
+      </c>
+      <c r="F9">
         <v>0.66693318927175926</v>
       </c>
-      <c r="G8">
+      <c r="G9">
         <v>0.56134184814611221</v>
       </c>
-      <c r="H8">
+      <c r="H9">
         <v>0.66055949079149767</v>
       </c>
-      <c r="I8">
+      <c r="I9">
         <v>0.65724787719077571</v>
       </c>
-      <c r="J8">
+      <c r="J9">
         <v>0.64701382882915426</v>
       </c>
-      <c r="K8">
+      <c r="K9">
+        <v>0.70087846409313204</v>
+      </c>
+      <c r="L9">
         <v>4.1801275510204094</v>
-      </c>
-    </row>
-    <row r="14" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="M14" t="e">
-        <f>M2:M7</f>
-        <v>#VALUE!</v>
       </c>
     </row>
   </sheetData>
@@ -739,13 +805,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="N8" sqref="N8"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="M1" sqref="M1:N8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>7</v>
       </c>
@@ -774,7 +840,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>8</v>
       </c>
@@ -815,7 +881,7 @@
         <v>11.5</v>
       </c>
     </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>9</v>
       </c>
@@ -859,7 +925,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>10</v>
       </c>
@@ -903,7 +969,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>11</v>
       </c>
@@ -947,7 +1013,7 @@
         <v>10.5</v>
       </c>
     </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>20</v>
       </c>
@@ -991,7 +1057,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="7" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>12</v>
       </c>
@@ -1035,7 +1101,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="8" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:14" x14ac:dyDescent="0.25">
       <c r="E8" t="s">
         <v>19</v>
       </c>
@@ -1067,7 +1133,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="9" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:14" x14ac:dyDescent="0.25">
       <c r="E9" t="s">
         <v>5</v>
       </c>
@@ -1103,20 +1169,26 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L9"/>
+  <dimension ref="A1:N9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D1" sqref="D1:D6"/>
+      <selection activeCell="N17" sqref="N17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>7</v>
       </c>
+      <c r="B1">
+        <v>59.35</v>
+      </c>
       <c r="C1" t="s">
         <v>13</v>
+      </c>
+      <c r="D1">
+        <v>47.825000000000152</v>
       </c>
       <c r="E1" s="1" t="s">
         <v>6</v>
@@ -1127,14 +1199,26 @@
       <c r="I1" s="1"/>
       <c r="J1" s="1"/>
       <c r="K1" s="1"/>
-    </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M1" t="s">
+        <v>22</v>
+      </c>
+      <c r="N1" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>8</v>
       </c>
+      <c r="B2">
+        <v>38.524999999999999</v>
+      </c>
       <c r="C2" t="s">
         <v>14</v>
       </c>
+      <c r="D2">
+        <v>8.5389030612244845</v>
+      </c>
       <c r="F2" t="s">
         <v>0</v>
       </c>
@@ -1156,187 +1240,289 @@
       <c r="L2" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M2" t="s">
+        <v>0</v>
+      </c>
+      <c r="N2">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>9</v>
       </c>
+      <c r="B3">
+        <v>26.25</v>
+      </c>
       <c r="C3" t="s">
         <v>15</v>
       </c>
+      <c r="D3">
+        <v>1.721938775510204</v>
+      </c>
       <c r="E3" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="F3">
+        <v>47.825000000000152</v>
+      </c>
+      <c r="G3">
+        <v>0.89860195859160907</v>
+      </c>
+      <c r="H3">
+        <v>0.39055613946699108</v>
+      </c>
+      <c r="I3">
+        <v>0.88065519862152442</v>
+      </c>
+      <c r="J3">
+        <v>0.7674980326058658</v>
+      </c>
+      <c r="K3">
+        <v>0.95571703716127399</v>
+      </c>
+      <c r="L3">
+        <v>0.73333147463748849</v>
+      </c>
+      <c r="M3" t="s">
+        <v>1</v>
+      </c>
+      <c r="N3">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>10</v>
       </c>
+      <c r="B4">
+        <v>37.104999999999997</v>
+      </c>
       <c r="C4" t="s">
         <v>16</v>
       </c>
+      <c r="D4">
+        <v>8.4874744897959129</v>
+      </c>
       <c r="E4" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="F4">
+        <v>0.89860195859160907</v>
+      </c>
+      <c r="G4">
+        <v>8.5389030612244845</v>
+      </c>
+      <c r="H4">
+        <v>0.41912598580676169</v>
+      </c>
+      <c r="I4">
+        <v>0.8833722729119432</v>
+      </c>
+      <c r="J4">
+        <v>0.81716128746184091</v>
+      </c>
+      <c r="K4">
+        <v>0.91173449989318855</v>
+      </c>
+      <c r="L4">
+        <v>0.58295055730360978</v>
+      </c>
+      <c r="M4" t="s">
+        <v>2</v>
+      </c>
+      <c r="N4">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>11</v>
       </c>
+      <c r="B5">
+        <v>33.195</v>
+      </c>
       <c r="C5" t="s">
         <v>17</v>
       </c>
+      <c r="D5">
+        <v>5.3400255102040788</v>
+      </c>
       <c r="E5" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="F5">
+        <v>0.39055613946699108</v>
+      </c>
+      <c r="G5">
+        <v>0.41912598580676169</v>
+      </c>
+      <c r="H5">
+        <v>1.721938775510204</v>
+      </c>
+      <c r="I5">
+        <v>0.45542670701031968</v>
+      </c>
+      <c r="J5">
+        <v>0.43535523225899375</v>
+      </c>
+      <c r="K5">
+        <v>0.4639832594792308</v>
+      </c>
+      <c r="L5">
+        <v>0.299375019665579</v>
+      </c>
+      <c r="M5" t="s">
+        <v>3</v>
+      </c>
+      <c r="N5">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>12</v>
+        <v>20</v>
+      </c>
+      <c r="B6">
+        <v>46.045000000000002</v>
       </c>
       <c r="C6" t="s">
-        <v>18</v>
+        <v>21</v>
+      </c>
+      <c r="D6">
+        <v>17.205841836734724</v>
       </c>
       <c r="E6" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="F6">
+        <v>0.88065519862152442</v>
+      </c>
+      <c r="G6">
+        <v>0.8833722729119432</v>
+      </c>
+      <c r="H6">
+        <v>0.45542670701031968</v>
+      </c>
+      <c r="I6">
+        <v>8.4874744897959129</v>
+      </c>
+      <c r="J6">
+        <v>0.89532729859337834</v>
+      </c>
+      <c r="K6">
+        <v>0.94089266153255813</v>
+      </c>
+      <c r="L6">
+        <v>0.62216245119326885</v>
+      </c>
+      <c r="M6" t="s">
+        <v>4</v>
+      </c>
+      <c r="N6">
+        <v>11.5</v>
+      </c>
+    </row>
+    <row r="7" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>12</v>
+      </c>
+      <c r="B7">
+        <v>32.61</v>
+      </c>
+      <c r="C7" t="s">
+        <v>18</v>
+      </c>
+      <c r="D7">
+        <v>4.1840816326530641</v>
+      </c>
       <c r="E7" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="F7">
+        <v>0.7674980326058658</v>
+      </c>
+      <c r="G7">
+        <v>0.81716128746184091</v>
+      </c>
+      <c r="H7">
+        <v>0.43535523225899375</v>
+      </c>
+      <c r="I7">
+        <v>0.89532729859337834</v>
+      </c>
+      <c r="J7">
+        <v>5.3400255102040788</v>
+      </c>
+      <c r="K7">
+        <v>0.92309149730730422</v>
+      </c>
+      <c r="L7">
+        <v>0.59927956370706503</v>
+      </c>
+      <c r="M7" t="s">
+        <v>19</v>
+      </c>
+      <c r="N7">
+        <v>6.5</v>
+      </c>
+    </row>
+    <row r="8" spans="1:14" x14ac:dyDescent="0.25">
       <c r="E8" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="F8">
+        <v>0.95571703716127399</v>
+      </c>
+      <c r="G8">
+        <v>0.91173449989318855</v>
+      </c>
+      <c r="H8">
+        <v>0.4639832594792308</v>
+      </c>
+      <c r="I8">
+        <v>0.94089266153255813</v>
+      </c>
+      <c r="J8">
+        <v>0.92309149730730422</v>
+      </c>
+      <c r="K8">
+        <v>17.205841836734724</v>
+      </c>
+      <c r="L8">
+        <v>0.62086925929687897</v>
+      </c>
+      <c r="M8" t="s">
+        <v>5</v>
+      </c>
+      <c r="N8">
+        <v>11.5</v>
+      </c>
+    </row>
+    <row r="9" spans="1:14" x14ac:dyDescent="0.25">
       <c r="E9" t="s">
         <v>5</v>
       </c>
-    </row>
-  </sheetData>
-  <mergeCells count="1">
-    <mergeCell ref="E1:K1"/>
-  </mergeCells>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L9"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E2" sqref="E2:L9"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A1" t="s">
-        <v>7</v>
-      </c>
-      <c r="C1" t="s">
-        <v>13</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="F1" s="1"/>
-      <c r="G1" s="1"/>
-      <c r="H1" s="1"/>
-      <c r="I1" s="1"/>
-      <c r="J1" s="1"/>
-      <c r="K1" s="1"/>
-    </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A2" t="s">
-        <v>8</v>
-      </c>
-      <c r="C2" t="s">
-        <v>14</v>
-      </c>
-      <c r="F2" t="s">
-        <v>0</v>
-      </c>
-      <c r="G2" t="s">
-        <v>1</v>
-      </c>
-      <c r="H2" t="s">
-        <v>2</v>
-      </c>
-      <c r="I2" t="s">
-        <v>3</v>
-      </c>
-      <c r="J2" t="s">
-        <v>4</v>
-      </c>
-      <c r="K2" t="s">
-        <v>19</v>
-      </c>
-      <c r="L2" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A3" t="s">
-        <v>9</v>
-      </c>
-      <c r="C3" t="s">
-        <v>15</v>
-      </c>
-      <c r="E3" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A4" t="s">
-        <v>10</v>
-      </c>
-      <c r="C4" t="s">
-        <v>16</v>
-      </c>
-      <c r="E4" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A5" t="s">
-        <v>11</v>
-      </c>
-      <c r="C5" t="s">
-        <v>17</v>
-      </c>
-      <c r="E5" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A6" t="s">
-        <v>12</v>
-      </c>
-      <c r="C6" t="s">
-        <v>18</v>
-      </c>
-      <c r="E6" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="E7" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="E8" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="E9" t="s">
-        <v>5</v>
+      <c r="F9">
+        <v>0.73333147463748849</v>
+      </c>
+      <c r="G9">
+        <v>0.58295055730360978</v>
+      </c>
+      <c r="H9">
+        <v>0.299375019665579</v>
+      </c>
+      <c r="I9">
+        <v>0.62216245119326885</v>
+      </c>
+      <c r="J9">
+        <v>0.59927956370706503</v>
+      </c>
+      <c r="K9">
+        <v>0.62086925929687897</v>
+      </c>
+      <c r="L9">
+        <v>4.1840816326530641</v>
       </c>
     </row>
   </sheetData>

</xml_diff>